<commit_message>
Update summary of paper-excel version.xlsx
</commit_message>
<xml_diff>
--- a/summary of paper-excel version.xlsx
+++ b/summary of paper-excel version.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <r>
       <t>1.</t>
@@ -534,13 +534,90 @@
       </rPr>
       <t xml:space="preserve"> Improved performance of serially connected Li-ion batteries with active cell balancing in electric vehicles.</t>
     </r>
+  </si>
+  <si>
+    <t>Title: Development of BMS for EVs in Malaysia.</t>
+  </si>
+  <si>
+    <t>1.       Does paper target series or parallel batteries?</t>
+  </si>
+  <si>
+    <t>N/A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.       Does paper target charging, discharging, or both. </t>
+  </si>
+  <si>
+    <t>3.       Is author using active or passive technique?</t>
+  </si>
+  <si>
+    <t>Active.</t>
+  </si>
+  <si>
+    <t>4.       Which is the subcategory?</t>
+  </si>
+  <si>
+    <t>Bi-directional DC/DC converter+HV ultra-capacitor.</t>
+  </si>
+  <si>
+    <t>5.       Which parameter is being monitored for cell balancing?</t>
+  </si>
+  <si>
+    <t>6.       What are they proposing circuit, techniques, and algorithm?</t>
+  </si>
+  <si>
+    <t>Circuit+ EV schematic+ algorithm.</t>
+  </si>
+  <si>
+    <t>7.       What are components used?</t>
+  </si>
+  <si>
+    <t>8.       Is it physical experiment or simulation?</t>
+  </si>
+  <si>
+    <t>Proposed circuit configuration+proposed algorithm.</t>
+  </si>
+  <si>
+    <t>9.       If, simulation which tools are being used?</t>
+  </si>
+  <si>
+    <t>Matlab/Simulink.</t>
+  </si>
+  <si>
+    <t>10.   If hardware which components are being used?</t>
+  </si>
+  <si>
+    <t>Bi-directional DC/DC converter+Battery+HV ultra-capacitor.</t>
+  </si>
+  <si>
+    <t>11.   What are evaluation parameters? In other words what is recorded
+ during experiment what is the comparison benchmark?</t>
+  </si>
+  <si>
+    <t>12.   What are test conditions?</t>
+  </si>
+  <si>
+    <t>13.   What are final results?</t>
+  </si>
+  <si>
+    <t>HESS is the the future BMS which should integrate ultracapacitor combined with Li battery. Further improvements are
+required.</t>
+  </si>
+  <si>
+    <t>14.   What are the improvements compared to previous one?</t>
+  </si>
+  <si>
+    <t>15.   What is your opinion?</t>
+  </si>
+  <si>
+    <t>It is a review paper and does not provide details regarding the proposed technology. Further research is required.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,10 +701,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -636,6 +713,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -682,7 +767,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -714,9 +799,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -748,6 +834,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -923,14 +1010,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75.7109375" customWidth="1"/>
     <col min="2" max="2" width="115.5703125" customWidth="1"/>
@@ -938,13 +1025,13 @@
     <col min="6" max="6" width="73.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" ht="30" customHeight="1">
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -952,7 +1039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" customHeight="1">
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -960,7 +1047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" customHeight="1">
+    <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -968,7 +1055,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" customHeight="1">
+    <row r="5" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -976,7 +1063,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" customHeight="1">
+    <row r="6" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -984,7 +1071,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" customHeight="1">
+    <row r="7" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -992,7 +1079,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" customHeight="1">
+    <row r="8" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1000,7 +1087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" customHeight="1">
+    <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1008,7 +1095,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" customHeight="1">
+    <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1016,7 +1103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" customHeight="1">
+    <row r="11" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1024,7 +1111,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" customHeight="1">
+    <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
@@ -1032,7 +1119,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" customHeight="1">
+    <row r="13" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1040,7 +1127,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30" customHeight="1">
+    <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1048,7 +1135,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="30" customHeight="1">
+    <row r="15" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1056,7 +1143,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30" customHeight="1">
+    <row r="16" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1064,7 +1151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" ht="30" customHeight="1"/>
+    <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
@@ -1075,24 +1162,158 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.140625" customWidth="1"/>
+    <col min="2" max="2" width="101" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>